<commit_message>
test food source for YL
</commit_message>
<xml_diff>
--- a/TestA_MW.xlsx
+++ b/TestA_MW.xlsx
@@ -14,9 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Hello world</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>EX_glc_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_h2o_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_h_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_inost_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_k_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_na1_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_nh4_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_o2_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_pi_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>EX_so4_LPAREN_e_RPAREN_</t>
+  </si>
+  <si>
+    <t>trehalose_c_tp</t>
   </si>
 </sst>
 </file>
@@ -348,15 +378,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0.08000000000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>41.65422506566294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>41.65422506566294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>41.64483387653971</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>41.65422506566294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>41.65422506566294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>19.45251739130443</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.08000000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>19.45251739130411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>19.45251739130492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>41.65422506566343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>